<commit_message>
chore(refactor): refactoring of model files and utilities
</commit_message>
<xml_diff>
--- a/data/customers.xlsx
+++ b/data/customers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="225">
   <si>
     <t>email</t>
   </si>
@@ -304,7 +304,7 @@
     <t>07-04-2020</t>
   </si>
   <si>
-    <t>camila.cortes@example.com</t>
+    <t>camilo.cortes@example.com</t>
   </si>
   <si>
     <t>91234578</t>
@@ -316,7 +316,7 @@
     <t>30-03-1999</t>
   </si>
   <si>
-    <t>Camila</t>
+    <t>Camilo</t>
   </si>
   <si>
     <t>12-01-2021</t>
@@ -502,7 +502,7 @@
     <t>25-01-2021</t>
   </si>
   <si>
-    <t>javiera.sanchez@example.com</t>
+    <t>javier.sanchez@example.com</t>
   </si>
   <si>
     <t>91234588</t>
@@ -512,9 +512,6 @@
   </si>
   <si>
     <t>12-12-1998</t>
-  </si>
-  <si>
-    <t>Javiera</t>
   </si>
   <si>
     <t>06-08-2019</t>
@@ -1435,7 +1432,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>98</v>
@@ -1725,7 +1722,7 @@
         <v>163</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>164</v>
@@ -1734,7 +1731,7 @@
         <v>165</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>166</v>
+        <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>86</v>
@@ -1743,15 +1740,15 @@
         <v>33</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
@@ -1760,39 +1757,39 @@
         <v>37</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>93</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>147</v>
@@ -1801,15 +1798,15 @@
         <v>133</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
@@ -1818,10 +1815,10 @@
         <v>12</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>56</v>
@@ -1830,15 +1827,15 @@
         <v>71</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -1847,27 +1844,27 @@
         <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>11</v>
@@ -1876,27 +1873,27 @@
         <v>29</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>20</v>
@@ -1905,27 +1902,27 @@
         <v>37</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>120</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>11</v>
@@ -1934,27 +1931,27 @@
         <v>45</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>64</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -1963,10 +1960,10 @@
         <v>52</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>48</v>
@@ -1975,15 +1972,15 @@
         <v>78</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
@@ -1992,27 +1989,27 @@
         <v>60</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>63</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>20</v>
@@ -2021,19 +2018,19 @@
         <v>68</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>